<commit_message>
message to your submodule repo
</commit_message>
<xml_diff>
--- a/CoreJava/test.xlsx
+++ b/CoreJava/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BD162B0B-1540-4CCB-B4EE-2BF644E00D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9CE3DD72-BF21-4C72-9166-2DDD0155B76A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="29100" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,6 +374,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>